<commit_message>
add both low arms
</commit_message>
<xml_diff>
--- a/Calibration/Formulas.xlsx
+++ b/Calibration/Formulas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamr1\Documents\Maestria\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamr1\Documents\Maestria\Captoglove\GsdkNet_1.2.5\GsdkNet_1.2.5\2018\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="79">
   <si>
     <t>index</t>
   </si>
@@ -149,9 +149,6 @@
     <t>max guante</t>
   </si>
   <si>
-    <t>roll</t>
-  </si>
-  <si>
     <t>unity</t>
   </si>
   <si>
@@ -206,59 +203,78 @@
     <t>plana</t>
   </si>
   <si>
-    <t>quartenion</t>
-  </si>
-  <si>
     <t>YAW</t>
   </si>
   <si>
-    <t>x unity and glove</t>
-  </si>
-  <si>
-    <t>z unity y in glove</t>
-  </si>
-  <si>
     <t>ROLL</t>
   </si>
   <si>
-    <t>y unity z in glove</t>
-  </si>
-  <si>
-    <t>No limitations</t>
-  </si>
-  <si>
-    <t>Limitations</t>
-  </si>
-  <si>
     <t>LEFT HAND</t>
   </si>
   <si>
     <t>LOW ARM R</t>
   </si>
   <si>
-    <t>x unity y in glove</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pitch </t>
-  </si>
-  <si>
-    <t>glove</t>
-  </si>
-  <si>
-    <t>y unity and z in glove</t>
-  </si>
-  <si>
     <t>Para calibrar, tocar hombro opuesto y estirar brazo</t>
   </si>
   <si>
-    <t>hacia la izquierda se vuelve positivo</t>
+    <t>RIGHT HAND</t>
+  </si>
+  <si>
+    <t>PITCH</t>
+  </si>
+  <si>
+    <t>Unity axe</t>
+  </si>
+  <si>
+    <t>Glove axe</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Unity Min</t>
+  </si>
+  <si>
+    <t>Glove Min</t>
+  </si>
+  <si>
+    <t>Unity Max</t>
+  </si>
+  <si>
+    <t>Glove Max</t>
+  </si>
+  <si>
+    <t>QUARTENION 
+POSITIVO</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>LOW ARM L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,14 +306,21 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +330,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -334,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,7 +399,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,7 +463,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -437,17 +502,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja3!$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ROLL</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -458,32 +512,56 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja3!$B$15:$B$17</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="1">
-                  <c:v>x unity and glove</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>z unity y in glove</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja3!$B$18</c:f>
+              <c:f>Hoja3!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja3!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja3!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:strRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -495,11 +573,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="361991296"/>
-        <c:axId val="361990512"/>
+        <c:axId val="256579776"/>
+        <c:axId val="256580168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361991296"/>
+        <c:axId val="256579776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +620,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361990512"/>
+        <c:crossAx val="256580168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361990512"/>
+        <c:axId val="256580168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,7 +679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361991296"/>
+        <c:crossAx val="256579776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1439,11 +1517,11 @@
       <sheetName val="Hoja11"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6">
         <row r="4">
@@ -1469,10 +1547,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3188,7 +3266,7 @@
         <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -3207,10 +3285,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -3225,14 +3303,14 @@
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -3240,7 +3318,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>-80</v>
@@ -3272,10 +3350,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -3303,7 +3381,7 @@
         <v>45.380727786172464</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -3329,20 +3407,20 @@
         <v>85.31320573750051</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17">
         <v>-40</v>
@@ -3374,10 +3452,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>52</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="12"/>
@@ -3407,7 +3485,7 @@
         <v>-1.3976695630119582</v>
       </c>
       <c r="I21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3433,7 +3511,7 @@
         <v>-1.4878752759811462</v>
       </c>
       <c r="I22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -3441,7 +3519,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26">
         <v>30</v>
@@ -3465,10 +3543,10 @@
         <v>91.943849010771004</v>
       </c>
       <c r="I26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3476,10 +3554,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
         <v>56</v>
-      </c>
-      <c r="D27" t="s">
-        <v>57</v>
       </c>
       <c r="J27" s="11">
         <f>+AVERAGE([1]R_pitch!N25,[1]R_roll!$G$4,[1]R_yaw!$G$4,[1]R_pitch!N29,[1]R_roll!$G$10,[1]R_yaw!$G$8)</f>
@@ -3493,488 +3571,738 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E1" s="4"/>
+      <c r="F1" s="12"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <f>-180+M4</f>
+        <v>-180</v>
+      </c>
+      <c r="E4" s="4">
+        <f>180+M4</f>
+        <v>180</v>
+      </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <f>+(E4-D4)/(G4-F4)</f>
+        <v>180</v>
+      </c>
+      <c r="I4" s="4">
+        <f>+D4-H4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <f>180+M6</f>
+        <v>180</v>
+      </c>
+      <c r="E5" s="4">
+        <f>-180+M6</f>
+        <v>-180</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <f>+(E5-D5)/(G5-F5)</f>
+        <v>-180</v>
+      </c>
+      <c r="I5" s="4">
+        <f>+D5-H5*F5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5">
+        <v>90</v>
+      </c>
+      <c r="N5">
+        <v>3.780758E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="B6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <f>-180+M5</f>
+        <v>-90</v>
+      </c>
+      <c r="E6" s="4">
+        <f>180+M5</f>
+        <v>270</v>
+      </c>
+      <c r="F6">
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <f>+(E6-D6)/(G6-F6)</f>
+        <v>180</v>
+      </c>
+      <c r="I6" s="4">
+        <f>+D6-H6*F6</f>
+        <v>90</v>
+      </c>
+      <c r="J6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="23">
+        <v>-6.556511E-9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A9" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="J10" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11">
+        <f>180+M11</f>
         <v>180</v>
       </c>
-      <c r="E4" s="13">
-        <v>-92.704863044925048</v>
-      </c>
-      <c r="F4">
-        <v>36.49704536376619</v>
-      </c>
-      <c r="G4" s="4">
-        <f>+(D4-C4)/(F4-E4)</f>
-        <v>1.3931682760491768</v>
-      </c>
-      <c r="H4" s="4">
-        <f>+C4-G4*E4</f>
-        <v>129.15347422967326</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="12">
-        <v>-47.842209692412922</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="E11" s="4">
+        <f>-180+M11</f>
+        <v>-180</v>
+      </c>
+      <c r="F11">
+        <v>-1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <f>+(E11-D11)/(G11-F11)</f>
+        <v>-180</v>
+      </c>
+      <c r="I11" s="4">
+        <f>+D11-H11*F11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12">
+        <f>-180+M13</f>
+        <v>-180</v>
+      </c>
+      <c r="E12" s="4">
+        <f>180+M13</f>
+        <v>180</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <f>+(E12-D12)/(G12-F12)</f>
+        <v>180</v>
+      </c>
+      <c r="I12" s="4">
+        <f>+D12-H12*F12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>75</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12">
+        <v>-90</v>
+      </c>
+      <c r="N12">
+        <v>3.780758E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13">
+        <f>-180+M12</f>
+        <v>-270</v>
+      </c>
+      <c r="E13" s="4">
+        <f>180+M12</f>
+        <v>90</v>
+      </c>
+      <c r="F13">
+        <v>-1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <f>+(E13-D13)/(G13-F13)</f>
+        <v>180</v>
+      </c>
+      <c r="I13" s="4">
+        <f>+D13-H13*F13</f>
+        <v>-90</v>
+      </c>
+      <c r="J13" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="23">
+        <v>-6.556511E-9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A16" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D7" s="4"/>
-      <c r="E7" s="12"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="I17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N17" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="26">
+        <f>-180+M18</f>
+        <v>-180</v>
+      </c>
+      <c r="E18" s="27">
+        <f>180+M18</f>
+        <v>180</v>
+      </c>
+      <c r="F18" s="26">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="26">
+        <v>1</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" s="26">
+        <v>0</v>
+      </c>
+      <c r="N18" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19">
+        <f>180+M19</f>
+        <v>180</v>
+      </c>
+      <c r="E19" s="4">
+        <f>-180+M19</f>
+        <v>-180</v>
+      </c>
+      <c r="F19">
+        <v>-1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="4">
+        <f>+(E19-D19)/(G19-F19)</f>
+        <v>-180</v>
+      </c>
+      <c r="I19" s="4">
+        <f>+D19-H19*F19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>75</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>3.9789209999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <f>-180+M20</f>
+        <v>-180</v>
+      </c>
+      <c r="E20" s="4">
+        <f>180+M20</f>
+        <v>180</v>
+      </c>
+      <c r="F20">
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
+        <f>+(E20-D20)/(G20-F20)</f>
+        <v>180</v>
+      </c>
+      <c r="I20" s="4">
+        <f>+D20-H20*F20</f>
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>75</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A23" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9">
+      <c r="C24" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N24" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="26">
+        <f>-180+M25</f>
         <v>-180</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E25" s="27">
+        <f>180+M25</f>
         <v>180</v>
       </c>
-      <c r="E9">
+      <c r="F25" s="26">
         <v>-1</v>
       </c>
-      <c r="F9">
+      <c r="G25" s="26">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
-        <f>+(D9-C9)/(F9-E9)</f>
+      <c r="J25" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="M25" s="26">
+        <v>0</v>
+      </c>
+      <c r="N25" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26">
+        <f>180+M26</f>
         <v>180</v>
       </c>
-      <c r="H9" s="4">
-        <f>+C9-G9*E9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="E26" s="4">
+        <f>-180+M26</f>
+        <v>-180</v>
+      </c>
+      <c r="F26">
+        <v>-1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" s="4">
+        <f>+(E26-D26)/(G26-F26)</f>
+        <v>-180</v>
+      </c>
+      <c r="I26" s="4">
+        <f>+D26-H26*F26</f>
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>75</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>3.9789209999999998E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27">
+        <f>-180+M27</f>
+        <v>-180</v>
+      </c>
+      <c r="E27" s="4">
+        <f>180+M27</f>
+        <v>180</v>
+      </c>
+      <c r="F27">
+        <v>-1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="4">
+        <f>+(E27-D27)/(G27-F27)</f>
+        <v>180</v>
+      </c>
+      <c r="I27" s="4">
+        <f>+D27-H27*F27</f>
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>75</v>
+      </c>
+      <c r="L27" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>61</v>
       </c>
-      <c r="C10">
-        <v>-180</v>
-      </c>
-      <c r="D10" s="4">
-        <v>180</v>
-      </c>
-      <c r="E10">
-        <v>-1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <f>+(D10-C10)/(F10-E10)</f>
-        <v>180</v>
-      </c>
-      <c r="H10" s="4">
-        <f>+C10-G10*E10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11">
-        <v>-90</v>
-      </c>
-      <c r="D11">
-        <v>270</v>
-      </c>
-      <c r="E11">
-        <v>-1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <f>+(D11-C11)/(F11-E11)</f>
-        <v>180</v>
-      </c>
-      <c r="H11" s="4">
-        <f>+C11-G11*E11</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16">
-        <v>-90</v>
-      </c>
-      <c r="D16">
-        <v>90</v>
-      </c>
-      <c r="E16">
-        <v>-0.6</v>
-      </c>
-      <c r="F16">
-        <v>0.6</v>
-      </c>
-      <c r="G16" s="4">
-        <f>+(D16-C16)/(F16-E16)</f>
-        <v>150</v>
-      </c>
-      <c r="H16" s="4">
-        <f>+C16-G16*E16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17">
-        <v>-30</v>
-      </c>
-      <c r="D17">
-        <v>30</v>
-      </c>
-      <c r="E17">
-        <v>-0.25</v>
-      </c>
-      <c r="F17">
-        <v>0.25</v>
-      </c>
-      <c r="G17" s="4">
-        <f>+(D17-C17)/(F17-E17)</f>
-        <v>120</v>
-      </c>
-      <c r="H17" s="4">
-        <f>+C17-G17*E17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18">
-        <v>-90</v>
-      </c>
-      <c r="D18">
-        <v>180</v>
-      </c>
-      <c r="E18">
-        <v>-1</v>
-      </c>
-      <c r="F18">
-        <v>0.6</v>
-      </c>
-      <c r="G18" s="4">
-        <f>+(D18-C18)/(F18-E18)</f>
-        <v>168.75</v>
-      </c>
-      <c r="H18" s="4">
-        <f>+C18-G18*E18</f>
-        <v>78.75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23">
-        <v>180</v>
-      </c>
-      <c r="D23" s="4">
-        <v>-180</v>
-      </c>
-      <c r="E23">
-        <v>-1</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" s="4">
-        <f>+(D23-C23)/(F23-E23)</f>
-        <v>-180</v>
-      </c>
-      <c r="H23" s="4">
-        <f>+C23-G23*E23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24">
-        <v>-180</v>
-      </c>
-      <c r="D24" s="4">
-        <v>180</v>
-      </c>
-      <c r="E24">
-        <v>-1</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" s="4">
-        <f>+(D24-C24)/(F24-E24)</f>
-        <v>180</v>
-      </c>
-      <c r="H24" s="4">
-        <f>+C24-G24*E24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25">
-        <v>-270</v>
-      </c>
-      <c r="D25">
-        <v>90</v>
-      </c>
-      <c r="E25">
-        <v>-1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" s="4">
-        <f>+(D25-C25)/(F25-E25)</f>
-        <v>180</v>
-      </c>
-      <c r="H25" s="4">
-        <f>+C25-G25*E25</f>
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29">
-        <v>-180</v>
-      </c>
-      <c r="D29" s="4">
-        <v>180</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>-1</v>
-      </c>
-      <c r="G29" s="4">
-        <f>+(D29-C29)/(F29-E29)</f>
-        <v>-180</v>
-      </c>
-      <c r="H29" s="4">
-        <f>+C29-G29*E29</f>
-        <v>0</v>
-      </c>
-      <c r="J29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30">
-        <v>-180</v>
-      </c>
-      <c r="D30">
-        <v>180</v>
-      </c>
-      <c r="E30">
-        <v>-1</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" s="4">
-        <f>+(D30-C30)/(F30-E30)</f>
-        <v>180</v>
-      </c>
-      <c r="H30" s="4">
-        <f>+C30-G30*E30</f>
-        <v>0</v>
-      </c>
-      <c r="J30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>72</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O3:P3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Include pitch of up arm
</commit_message>
<xml_diff>
--- a/Calibration/Formulas.xlsx
+++ b/Calibration/Formulas.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="82">
   <si>
     <t>index</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>LOW ARM R</t>
-  </si>
-  <si>
-    <t>Para calibrar, tocar hombro opuesto y estirar brazo</t>
   </si>
   <si>
     <t>RIGHT HAND</t>
@@ -268,13 +265,25 @@
   </si>
   <si>
     <t>LOW ARM L</t>
+  </si>
+  <si>
+    <t>UP ARM L</t>
+  </si>
+  <si>
+    <t>disminyye</t>
+  </si>
+  <si>
+    <t>disminuye</t>
+  </si>
+  <si>
+    <t>UP ARM R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +324,19 @@
     <font>
       <sz val="11"/>
       <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -369,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,9 +438,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -431,6 +450,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,7 +577,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:strRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -557,7 +585,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:strRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -573,11 +601,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="256579776"/>
-        <c:axId val="256580168"/>
+        <c:axId val="265655856"/>
+        <c:axId val="156226256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256579776"/>
+        <c:axId val="265655856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,7 +648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256580168"/>
+        <c:crossAx val="156226256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -628,7 +656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256580168"/>
+        <c:axId val="156226256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256579776"/>
+        <c:crossAx val="265655856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3571,10 +3599,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3583,6 +3611,8 @@
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -3593,7 +3623,7 @@
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -3603,53 +3633,53 @@
     </row>
     <row r="3" spans="1:16" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>65</v>
-      </c>
       <c r="D3" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <f>-180+M4</f>
@@ -3674,10 +3704,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L4" s="24" t="s">
-        <v>66</v>
+        <v>73</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -3691,10 +3721,10 @@
         <v>57</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <f>180+M6</f>
@@ -3719,10 +3749,10 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>67</v>
+        <v>74</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>66</v>
       </c>
       <c r="M5">
         <v>90</v>
@@ -3736,10 +3766,10 @@
         <v>58</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D6">
         <f>-180+M5</f>
@@ -3764,67 +3794,104 @@
         <v>90</v>
       </c>
       <c r="J6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="22">
+        <v>-6.556511E-9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A8" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="23">
-        <v>-6.556511E-9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="N9" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="20" t="s">
+      <c r="D10" s="25">
+        <f>-180+M10</f>
+        <v>-180</v>
+      </c>
+      <c r="E10" s="26">
+        <f>180+M10</f>
+        <v>180</v>
+      </c>
+      <c r="F10" s="25">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="25">
+        <v>1</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L10" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>77</v>
+      <c r="L10" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" s="25">
+        <v>0</v>
+      </c>
+      <c r="N10" s="25">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>66</v>
@@ -3854,32 +3921,32 @@
       <c r="J11" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="L11" s="23" t="s">
         <v>66</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>3.9789209999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D12">
-        <f>-180+M13</f>
+        <f>-180+M12</f>
         <v>-180</v>
       </c>
       <c r="E12" s="4">
-        <f>180+M13</f>
+        <f>180+M12</f>
         <v>180</v>
       </c>
       <c r="F12">
@@ -3897,407 +3964,774 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A14" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="N15" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
         <v>67</v>
       </c>
-      <c r="M12">
+      <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16">
+        <v>90</v>
+      </c>
+      <c r="E16" s="4">
         <v>-90</v>
       </c>
-      <c r="N12">
+      <c r="F16">
+        <v>-1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <f>+(E16-D16)/(G16-F16)</f>
+        <v>-90</v>
+      </c>
+      <c r="I16" s="4">
+        <f>+D16-H16*F16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="M16">
+        <v>-100</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C17" s="1"/>
+      <c r="E17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="L17" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1.5894140000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C18" s="1"/>
+      <c r="E18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="L18" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A20" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22">
+        <f>180+M22</f>
+        <v>180</v>
+      </c>
+      <c r="E22" s="4">
+        <f>-180+M22</f>
+        <v>-180</v>
+      </c>
+      <c r="F22">
+        <v>-1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4">
+        <f>+(E22-D22)/(G22-F22)</f>
+        <v>-180</v>
+      </c>
+      <c r="I22" s="4">
+        <f>+D22-H22*F22</f>
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23">
+        <f>-180+M24</f>
+        <v>-180</v>
+      </c>
+      <c r="E23" s="4">
+        <f>180+M24</f>
+        <v>180</v>
+      </c>
+      <c r="F23">
+        <v>-1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4">
+        <f>+(E23-D23)/(G23-F23)</f>
+        <v>180</v>
+      </c>
+      <c r="I23" s="4">
+        <f>+D23-H23*F23</f>
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23">
+        <v>-90</v>
+      </c>
+      <c r="N23">
         <v>3.780758E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>58</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D24">
+        <f>-180+M23</f>
+        <v>-270</v>
+      </c>
+      <c r="E24" s="4">
+        <f>180+M23</f>
+        <v>90</v>
+      </c>
+      <c r="F24">
+        <v>-1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4">
+        <f>+(E24-D24)/(G24-F24)</f>
+        <v>180</v>
+      </c>
+      <c r="I24" s="4">
+        <f>+D24-H24*F24</f>
+        <v>-90</v>
+      </c>
+      <c r="J24" t="s">
+        <v>74</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="22">
+        <v>-6.556511E-9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A28" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D13">
-        <f>-180+M12</f>
-        <v>-270</v>
-      </c>
-      <c r="E13" s="4">
-        <f>180+M12</f>
+      <c r="E29" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N29" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="25">
+        <f>-180+M30</f>
+        <v>-180</v>
+      </c>
+      <c r="E30" s="26">
+        <f>180+M30</f>
+        <v>180</v>
+      </c>
+      <c r="F30" s="25">
+        <v>-1</v>
+      </c>
+      <c r="G30" s="25">
+        <v>1</v>
+      </c>
+      <c r="J30" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L30" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M30" s="25">
+        <v>0</v>
+      </c>
+      <c r="N30" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31">
+        <f>180+M31</f>
+        <v>180</v>
+      </c>
+      <c r="E31" s="4">
+        <f>-180+M31</f>
+        <v>-180</v>
+      </c>
+      <c r="F31">
+        <v>-1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4">
+        <f>+(E31-D31)/(G31-F31)</f>
+        <v>-180</v>
+      </c>
+      <c r="I31" s="4">
+        <f>+D31-H31*F31</f>
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>74</v>
+      </c>
+      <c r="L31" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>3.9789209999999998E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32">
+        <f>-180+M32</f>
+        <v>-180</v>
+      </c>
+      <c r="E32" s="4">
+        <f>180+M32</f>
+        <v>180</v>
+      </c>
+      <c r="F32">
+        <v>-1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="4">
+        <f>+(E32-D32)/(G32-F32)</f>
+        <v>180</v>
+      </c>
+      <c r="I32" s="4">
+        <f>+D32-H32*F32</f>
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L32" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A35" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K36" s="16"/>
+      <c r="L36" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N36" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37">
+        <v>-90</v>
+      </c>
+      <c r="E37" s="4">
         <v>90</v>
       </c>
-      <c r="F13">
+      <c r="F37">
         <v>-1</v>
       </c>
-      <c r="G13">
+      <c r="G37">
         <v>1</v>
       </c>
-      <c r="H13" s="4">
-        <f>+(E13-D13)/(G13-F13)</f>
+      <c r="H37" s="4">
+        <f>+(E37-D37)/(G37-F37)</f>
+        <v>90</v>
+      </c>
+      <c r="I37" s="4">
+        <f>+D37-H37*F37</f>
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>73</v>
+      </c>
+      <c r="L37" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="M37" s="29">
+        <v>80</v>
+      </c>
+      <c r="N37" s="29">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="31">
+        <f>-90+M37</f>
+        <v>-10</v>
+      </c>
+      <c r="E38" s="32">
+        <f>270+M37</f>
+        <v>350</v>
+      </c>
+      <c r="F38" s="31">
+        <v>-1</v>
+      </c>
+      <c r="G38" s="31">
+        <v>1</v>
+      </c>
+      <c r="H38" s="32">
+        <f>+(E38-D38)/(G38-F38)</f>
         <v>180</v>
       </c>
-      <c r="I13" s="4">
-        <f>+D13-H13*F13</f>
-        <v>-90</v>
-      </c>
-      <c r="J13" t="s">
-        <v>75</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" s="23">
-        <v>-6.556511E-9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="16" t="s">
+      <c r="I38" s="32">
+        <f>+D38-H38*F38</f>
+        <v>170</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" s="31"/>
+      <c r="L38" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="M38" s="29">
+        <v>180</v>
+      </c>
+      <c r="N38" s="29">
+        <v>1.5894140000000001E-2</v>
+      </c>
+      <c r="O38" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="P38" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="31">
+        <v>360</v>
+      </c>
+      <c r="E39" s="32">
+        <v>0</v>
+      </c>
+      <c r="F39" s="31">
+        <v>-1</v>
+      </c>
+      <c r="G39" s="31">
+        <v>1</v>
+      </c>
+      <c r="H39" s="32">
+        <f>+(E39-D39)/(G39-F39)</f>
+        <v>-180</v>
+      </c>
+      <c r="I39" s="32">
+        <f>+D39-H39*F39</f>
+        <v>180</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="K39" s="31"/>
+      <c r="L39" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="M39" s="29">
+        <v>180</v>
+      </c>
+      <c r="N39" s="29">
+        <v>0</v>
+      </c>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31">
+        <f>+P38*H39+I39</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="L17" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="N17" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="26">
-        <f>-180+M18</f>
-        <v>-180</v>
-      </c>
-      <c r="E18" s="27">
-        <f>180+M18</f>
-        <v>180</v>
-      </c>
-      <c r="F18" s="26">
+      <c r="C40" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="32">
+        <v>-80</v>
+      </c>
+      <c r="E40" s="32">
+        <v>-80</v>
+      </c>
+      <c r="F40" s="31">
         <v>-1</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G40" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="L18" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="M18" s="26">
-        <v>0</v>
-      </c>
-      <c r="N18" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="H40" s="32">
+        <f>+(E40-D40)/(G40-F40)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="32">
+        <f>+D40-H40*F40</f>
+        <v>-80</v>
+      </c>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31">
+        <f>+P38*H40+I40+80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="31"/>
+      <c r="B41" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D19">
-        <f>180+M19</f>
-        <v>180</v>
-      </c>
-      <c r="E19" s="4">
-        <f>-180+M19</f>
-        <v>-180</v>
-      </c>
-      <c r="F19">
+      <c r="C41" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="31">
+        <v>-200</v>
+      </c>
+      <c r="E41" s="31">
+        <v>200</v>
+      </c>
+      <c r="F41" s="31">
         <v>-1</v>
       </c>
-      <c r="G19">
+      <c r="G41" s="31">
         <v>1</v>
       </c>
-      <c r="H19" s="4">
-        <f>+(E19-D19)/(G19-F19)</f>
-        <v>-180</v>
-      </c>
-      <c r="I19" s="4">
-        <f>+D19-H19*F19</f>
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>75</v>
-      </c>
-      <c r="L19" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>3.9789209999999998E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20">
-        <f>-180+M20</f>
-        <v>-180</v>
-      </c>
-      <c r="E20" s="4">
-        <f>180+M20</f>
-        <v>180</v>
-      </c>
-      <c r="F20">
-        <v>-1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4">
-        <f>+(E20-D20)/(G20-F20)</f>
-        <v>180</v>
-      </c>
-      <c r="I20" s="4">
-        <f>+D20-H20*F20</f>
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>75</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="A23" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="L24" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="N24" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="26">
-        <f>-180+M25</f>
-        <v>-180</v>
-      </c>
-      <c r="E25" s="27">
-        <f>180+M25</f>
-        <v>180</v>
-      </c>
-      <c r="F25" s="26">
-        <v>-1</v>
-      </c>
-      <c r="G25" s="26">
-        <v>1</v>
-      </c>
-      <c r="J25" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="L25" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="M25" s="26">
-        <v>0</v>
-      </c>
-      <c r="N25" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26">
-        <f>180+M26</f>
-        <v>180</v>
-      </c>
-      <c r="E26" s="4">
-        <f>-180+M26</f>
-        <v>-180</v>
-      </c>
-      <c r="F26">
-        <v>-1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26" s="4">
-        <f>+(E26-D26)/(G26-F26)</f>
-        <v>-180</v>
-      </c>
-      <c r="I26" s="4">
-        <f>+D26-H26*F26</f>
-        <v>0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>75</v>
-      </c>
-      <c r="L26" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>3.9789209999999998E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27">
-        <f>-180+M27</f>
-        <v>-180</v>
-      </c>
-      <c r="E27" s="4">
-        <f>180+M27</f>
-        <v>180</v>
-      </c>
-      <c r="F27">
-        <v>-1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4">
-        <f>+(E27-D27)/(G27-F27)</f>
-        <v>180</v>
-      </c>
-      <c r="I27" s="4">
-        <f>+D27-H27*F27</f>
-        <v>0</v>
-      </c>
-      <c r="J27" t="s">
-        <v>75</v>
-      </c>
-      <c r="L27" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>61</v>
-      </c>
+      <c r="H41" s="32">
+        <f>+(E41-D41)/(G41-F41)</f>
+        <v>200</v>
+      </c>
+      <c r="I41" s="32">
+        <f>+D41-H41*F41</f>
+        <v>0</v>
+      </c>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31">
+        <f>+P38*H41+I41</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
include formules for fingers
</commit_message>
<xml_diff>
--- a/Calibration/Formulas.xlsx
+++ b/Calibration/Formulas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="69">
   <si>
     <t>index</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>idx1</t>
-  </si>
-  <si>
-    <t>idx3</t>
   </si>
   <si>
     <t>La posicion natural es de aproximadamene -23 en el indice</t>
@@ -167,6 +164,75 @@
   </si>
   <si>
     <t>Limit in 0. After this the movement is of uparm</t>
+  </si>
+  <si>
+    <t>Read register SensorDescriptor (4161): (Tag = 0, Min = 55.675, Max = 8008.68, Hyst. = 1, ConfTime = 0.12, FilterFactor = 0.4)</t>
+  </si>
+  <si>
+    <t>Read register SensorDescriptor (4193): (Tag = 0, Min = 144.9752, Max = 3964.584, Hyst. = 1, ConfTime = 0.12, FilterFactor = 0.4)</t>
+  </si>
+  <si>
+    <t>Read register SensorDescriptor (4225): (Tag = 0, Min = 0, Max = 5768.436, Hyst. = 1, ConfTime = 0.12, FilterFactor = 0.4)</t>
+  </si>
+  <si>
+    <t>Read register SensorDescriptor (4257): (Tag = 0, Min = 127.4413, Max = 5252.221, Hyst. = 1, ConfTime = 0.12, FilterFactor = 0.4)</t>
+  </si>
+  <si>
+    <t>Read register SensorDescriptor (4289): (Tag = 0, Min = 0, Max = 2172.413, Hyst. = 1, ConfTime = 0.12, FilterFactor = 0.4)</t>
+  </si>
+  <si>
+    <t>thumb</t>
+  </si>
+  <si>
+    <t>idx</t>
+  </si>
+  <si>
+    <t>middle</t>
+  </si>
+  <si>
+    <t>pinky</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>Right hand</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Finger</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Pinkky</t>
+  </si>
+  <si>
+    <t>thum pressuere</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>Estos valores no son acertados, en espacial los máximos</t>
+  </si>
+  <si>
+    <t>012</t>
   </si>
 </sst>
 </file>
@@ -174,9 +240,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,14 +252,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -294,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,7 +370,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,37 +377,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -359,7 +413,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -429,8 +492,8 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>153363</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>30479</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -467,8 +530,8 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>557899</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>160019</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -499,13 +562,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>568436</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>212645</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -537,14 +600,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>43104</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>213216</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>139776</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -563,6 +626,82 @@
         <a:xfrm>
           <a:off x="8382000" y="8646084"/>
           <a:ext cx="3329796" cy="871296"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1755993</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>150325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3855720" y="4648200"/>
+          <a:ext cx="3333333" cy="1361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>496785</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>3617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="213360" y="4503420"/>
+          <a:ext cx="3361905" cy="1542857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -837,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,7 +990,7 @@
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
@@ -865,15 +1004,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -916,25 +1063,29 @@
         <v>0</v>
       </c>
       <c r="F7" s="6">
-        <v>80</v>
-      </c>
-      <c r="G7">
-        <v>3364.6990000000001</v>
-      </c>
-      <c r="H7">
-        <v>58.804519999999997</v>
+        <v>-80</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4527.6970000000001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>360.22140000000002</v>
       </c>
       <c r="I7" s="4">
         <f>+(F7-E7)/(H7-G7)</f>
-        <v>-2.4199199485641174E-2</v>
+        <v>1.9196273158743869E-2</v>
       </c>
       <c r="J7" s="4">
         <f>+E7-I7*G7</f>
-        <v>81.42302231013737</v>
+        <v>-86.91490839202514</v>
       </c>
       <c r="K7">
         <v>1698.499</v>
       </c>
+      <c r="L7">
+        <f>1000*I7+J7</f>
+        <v>-67.718635233281276</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -952,24 +1103,24 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="5">
-        <v>80</v>
+      <c r="F8" s="6">
+        <v>-80</v>
       </c>
       <c r="G8" s="4">
         <f>+G7</f>
-        <v>3364.6990000000001</v>
+        <v>4527.6970000000001</v>
       </c>
       <c r="H8" s="4">
         <f>+H7</f>
-        <v>58.804519999999997</v>
+        <v>360.22140000000002</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" ref="I8:I19" si="0">+(F8-E8)/(H8-G8)</f>
-        <v>-2.4199199485641174E-2</v>
+        <v>1.9196273158743869E-2</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" ref="J8:J21" si="1">+E8-I8*G8</f>
-        <v>81.42302231013737</v>
+        <v>-86.91490839202514</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -988,24 +1139,24 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="5">
-        <v>80</v>
+      <c r="F9" s="6">
+        <v>-80</v>
       </c>
       <c r="G9" s="4">
         <f>+G8</f>
-        <v>3364.6990000000001</v>
+        <v>4527.6970000000001</v>
       </c>
       <c r="H9" s="4">
         <f>+H8</f>
-        <v>58.804519999999997</v>
+        <v>360.22140000000002</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" si="0"/>
-        <v>-2.4199199485641174E-2</v>
+        <v>1.9196273158743869E-2</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="1"/>
-        <v>81.42302231013737</v>
+        <v>-86.91490839202514</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1025,21 +1176,21 @@
         <v>0</v>
       </c>
       <c r="F10" s="6">
-        <v>80</v>
+        <v>-80</v>
       </c>
       <c r="G10" s="4">
-        <v>5547.451</v>
+        <v>6164.5010000000002</v>
       </c>
       <c r="H10" s="4">
-        <v>500.11779999999999</v>
+        <v>831.02200000000005</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="0"/>
-        <v>-1.5849954189669904E-2</v>
+        <v>1.4999590323689284E-2</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="1"/>
-        <v>87.926844219438493</v>
+        <v>-92.464989549972913</v>
       </c>
       <c r="K10">
         <v>1026.175</v>
@@ -1061,24 +1212,24 @@
       <c r="E11" s="4">
         <v>0</v>
       </c>
-      <c r="F11" s="5">
-        <v>80</v>
+      <c r="F11" s="6">
+        <v>-80</v>
       </c>
       <c r="G11" s="4">
         <f>+G10</f>
-        <v>5547.451</v>
+        <v>6164.5010000000002</v>
       </c>
       <c r="H11" s="4">
         <f>+H10</f>
-        <v>500.11779999999999</v>
+        <v>831.02200000000005</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="0"/>
-        <v>-1.5849954189669904E-2</v>
+        <v>1.4999590323689284E-2</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="1"/>
-        <v>87.926844219438493</v>
+        <v>-92.464989549972913</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1097,24 +1248,24 @@
       <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="5">
-        <v>80</v>
+      <c r="F12" s="6">
+        <v>-80</v>
       </c>
       <c r="G12" s="4">
         <f>+G11</f>
-        <v>5547.451</v>
+        <v>6164.5010000000002</v>
       </c>
       <c r="H12" s="4">
         <f>+H11</f>
-        <v>500.11779999999999</v>
+        <v>831.02200000000005</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="0"/>
-        <v>-1.5849954189669904E-2</v>
+        <v>1.4999590323689284E-2</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="1"/>
-        <v>87.926844219438493</v>
+        <v>-92.464989549972913</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1134,21 +1285,21 @@
         <v>0</v>
       </c>
       <c r="F13" s="6">
-        <v>80</v>
-      </c>
-      <c r="G13">
-        <v>5928.3429999999998</v>
-      </c>
-      <c r="H13">
-        <v>125.46559999999999</v>
+        <v>-80</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5482.8209999999999</v>
+      </c>
+      <c r="H13" s="1">
+        <v>451.81880000000001</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="0"/>
-        <v>-1.3786264035149185E-2</v>
+        <f>+(F13-E13)/(H13-G13)</f>
+        <v>1.5901404296742309E-2</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="1"/>
-        <v>81.729701888928417</v>
+        <v>-87.184553407668957</v>
       </c>
       <c r="K13">
         <v>1071.23</v>
@@ -1170,24 +1321,24 @@
       <c r="E14" s="4">
         <v>0</v>
       </c>
-      <c r="F14" s="5">
-        <v>80</v>
+      <c r="F14" s="6">
+        <v>-80</v>
       </c>
       <c r="G14" s="4">
         <f>+G13</f>
-        <v>5928.3429999999998</v>
+        <v>5482.8209999999999</v>
       </c>
       <c r="H14" s="4">
         <f>+H13</f>
-        <v>125.46559999999999</v>
+        <v>451.81880000000001</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="0"/>
-        <v>-1.3786264035149185E-2</v>
+        <v>1.5901404296742309E-2</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="1"/>
-        <v>81.729701888928417</v>
+        <v>-87.184553407668957</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1206,24 +1357,24 @@
       <c r="E15" s="4">
         <v>0</v>
       </c>
-      <c r="F15" s="5">
-        <v>80</v>
+      <c r="F15" s="6">
+        <v>-80</v>
       </c>
       <c r="G15" s="4">
         <f>+G14</f>
-        <v>5928.3429999999998</v>
+        <v>5482.8209999999999</v>
       </c>
       <c r="H15" s="4">
         <f>+H14</f>
-        <v>125.46559999999999</v>
+        <v>451.81880000000001</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="0"/>
-        <v>-1.3786264035149185E-2</v>
+        <v>1.5901404296742309E-2</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="1"/>
-        <v>81.729701888928417</v>
+        <v>-87.184553407668957</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1243,24 +1394,28 @@
         <v>0</v>
       </c>
       <c r="F16" s="6">
-        <v>80</v>
-      </c>
-      <c r="G16">
-        <v>3377.8679999999999</v>
-      </c>
-      <c r="H16">
-        <v>86.231129999999993</v>
+        <v>-80</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5701.2309999999998</v>
+      </c>
+      <c r="H16" s="1">
+        <v>496.22590000000002</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" si="0"/>
-        <v>-2.4304017472012336E-2</v>
+        <v>1.5369821635717516E-2</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="1"/>
-        <v>82.095762890151363</v>
+        <v>-87.626903574023402</v>
       </c>
       <c r="K16">
         <v>1247.5119999999999</v>
+      </c>
+      <c r="L16">
+        <f>4474*I16+J16</f>
+        <v>-18.862321575823231</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1279,24 +1434,24 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="F17" s="5">
-        <v>80</v>
+      <c r="F17" s="6">
+        <v>-80</v>
       </c>
       <c r="G17" s="4">
         <f>+G16</f>
-        <v>3377.8679999999999</v>
+        <v>5701.2309999999998</v>
       </c>
       <c r="H17" s="4">
         <f>+H16</f>
-        <v>86.231129999999993</v>
+        <v>496.22590000000002</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" si="0"/>
-        <v>-2.4304017472012336E-2</v>
+        <v>1.5369821635717516E-2</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="1"/>
-        <v>82.095762890151363</v>
+        <v>-87.626903574023402</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1315,24 +1470,24 @@
       <c r="E18" s="4">
         <v>0</v>
       </c>
-      <c r="F18" s="5">
-        <v>80</v>
+      <c r="F18" s="6">
+        <v>-80</v>
       </c>
       <c r="G18" s="4">
         <f>+G17</f>
-        <v>3377.8679999999999</v>
+        <v>5701.2309999999998</v>
       </c>
       <c r="H18" s="4">
         <f>+H17</f>
-        <v>86.231129999999993</v>
+        <v>496.22590000000002</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" si="0"/>
-        <v>-2.4304017472012336E-2</v>
+        <v>1.5369821635717516E-2</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="1"/>
-        <v>82.095762890151363</v>
+        <v>-87.626903574023402</v>
       </c>
       <c r="K18">
         <f>+AVERAGE(K7:K17)</f>
@@ -1361,19 +1516,19 @@
       <c r="F19" s="5">
         <v>30</v>
       </c>
-      <c r="G19">
-        <v>2672.114</v>
-      </c>
-      <c r="H19">
-        <v>1391.7</v>
+      <c r="G19" s="1">
+        <v>5011.7039999999997</v>
+      </c>
+      <c r="H19" s="4">
+        <v>315.42039999999997</v>
       </c>
       <c r="I19" s="4">
         <f t="shared" si="0"/>
-        <v>-3.1239895846187249E-2</v>
+        <v>-8.5173731841918579E-3</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="1"/>
-        <v>73.47656304913879</v>
+        <v>32.686553256707072</v>
       </c>
       <c r="K19">
         <v>3444.49</v>
@@ -1398,21 +1553,21 @@
       <c r="F20" s="5">
         <v>50</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <f>+G19</f>
-        <v>2672.114</v>
-      </c>
-      <c r="H20" s="4">
+        <v>5011.7039999999997</v>
+      </c>
+      <c r="H20" s="1">
         <f>+H19</f>
-        <v>1391.7</v>
+        <v>315.42039999999997</v>
       </c>
       <c r="I20" s="4">
         <f>+(F20-E20)/(H20-G20)</f>
-        <v>-3.9049869807734061E-2</v>
+        <v>-1.0646716480239822E-2</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="1"/>
-        <v>104.34570381142349</v>
+        <v>53.358191570883832</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1434,24 +1589,24 @@
       <c r="F21" s="5">
         <v>30</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <f>+G20</f>
-        <v>2672.114</v>
-      </c>
-      <c r="H21" s="4">
+        <v>5011.7039999999997</v>
+      </c>
+      <c r="H21" s="1">
         <f>+H20</f>
-        <v>1391.7</v>
+        <v>315.42039999999997</v>
       </c>
       <c r="I21" s="4">
         <f>+(F21-E21)/(H21-G21)</f>
-        <v>-2.3429921884640437E-2</v>
+        <v>-6.3880298881438934E-3</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="1"/>
-        <v>62.607422286854096</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>32.014914942530304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
@@ -1471,7 +1626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -1505,7 +1660,7 @@
         <v>89.890347929584237</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1524,11 +1679,11 @@
       <c r="F25" s="5">
         <v>80</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <f>+G24</f>
         <v>6460.3419999999996</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="1">
         <f>+H24</f>
         <v>710.81079999999997</v>
       </c>
@@ -1541,7 +1696,7 @@
         <v>89.890347929584237</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1564,7 +1719,7 @@
         <f>+G25</f>
         <v>6460.3419999999996</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <f>+H25</f>
         <v>710.81079999999997</v>
       </c>
@@ -1577,7 +1732,7 @@
         <v>89.890347929584237</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1599,19 +1754,19 @@
       <c r="G27" s="4">
         <v>5723.5450000000001</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="1">
         <v>0</v>
       </c>
       <c r="I27" s="4">
         <f t="shared" si="2"/>
         <v>-1.3977351449145591E-2</v>
       </c>
-      <c r="J27" s="24">
+      <c r="J27" s="22">
         <f>+E27-I27*G27</f>
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1634,19 +1789,19 @@
         <f>+G27</f>
         <v>5723.5450000000001</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1">
         <v>0</v>
       </c>
       <c r="I28" s="4">
         <f t="shared" si="2"/>
         <v>-1.3977351449145591E-2</v>
       </c>
-      <c r="J28" s="24">
+      <c r="J28" s="22">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1669,19 +1824,19 @@
         <f>+G28</f>
         <v>5723.5450000000001</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="1">
         <v>0</v>
       </c>
       <c r="I29" s="4">
         <f t="shared" si="2"/>
         <v>-1.3977351449145591E-2</v>
       </c>
-      <c r="J29" s="24">
+      <c r="J29" s="22">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1700,22 +1855,22 @@
       <c r="F30" s="6">
         <v>80</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>4545.4179999999997</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="1">
         <v>0</v>
       </c>
       <c r="I30" s="4">
         <f t="shared" si="2"/>
         <v>-1.7600141505137702E-2</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="22">
         <f>+E30-I30*G30</f>
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>7</v>
       </c>
@@ -1738,19 +1893,19 @@
         <f>+G30</f>
         <v>4545.4179999999997</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="1">
         <v>0</v>
       </c>
       <c r="I31" s="4">
         <f t="shared" si="2"/>
         <v>-1.7600141505137702E-2</v>
       </c>
-      <c r="J31" s="24">
+      <c r="J31" s="22">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8</v>
       </c>
@@ -1773,14 +1928,14 @@
         <f>+G31</f>
         <v>4545.4179999999997</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="1">
         <v>0</v>
       </c>
       <c r="I32" s="4">
         <f t="shared" si="2"/>
         <v>-1.7600141505137702E-2</v>
       </c>
-      <c r="J32" s="24">
+      <c r="J32" s="22">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
@@ -1788,7 +1943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>9</v>
       </c>
@@ -1807,10 +1962,10 @@
       <c r="F33" s="6">
         <v>80</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>6587.7610000000004</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <v>179.72110000000001</v>
       </c>
       <c r="I33" s="4">
@@ -1822,7 +1977,7 @@
         <v>82.243695143034287</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1858,7 +2013,7 @@
         <v>82.243695143034287</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>11</v>
       </c>
@@ -1894,7 +2049,7 @@
         <v>82.243695143034287</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>12</v>
       </c>
@@ -1913,10 +2068,10 @@
       <c r="F36" s="5">
         <v>30</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>5525.8230000000003</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="1">
         <v>960.2441</v>
       </c>
       <c r="I36" s="4">
@@ -1928,7 +2083,7 @@
         <v>38.412901154769223</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>13</v>
       </c>
@@ -1964,7 +2119,7 @@
         <v>60.516126443461523</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>14</v>
       </c>
@@ -2000,37 +2155,68 @@
         <v>36.309675866076915</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K41" s="1"/>
-      <c r="M41" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
       <c r="C43" s="3"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
       <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="5"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
@@ -2040,110 +2226,154 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C46" s="3"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C49" s="3"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-    </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-    </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C52" s="3"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="7"/>
-    </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-    </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C55" s="3"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="5"/>
-    </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-    </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F52" t="s">
+        <v>59</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>9</v>
+      </c>
+      <c r="H53" s="1">
+        <v>121314</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>61</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55" s="1">
+        <v>7</v>
+      </c>
+      <c r="H55" s="1">
+        <v>91011</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>62</v>
+      </c>
+      <c r="E56">
+        <v>5</v>
+      </c>
+      <c r="F56">
+        <v>4</v>
+      </c>
+      <c r="G56" s="1">
+        <v>5</v>
+      </c>
+      <c r="H56" s="1">
+        <v>6789</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57">
+        <v>7</v>
+      </c>
+      <c r="F57">
+        <v>6</v>
+      </c>
+      <c r="G57" s="1">
+        <v>3</v>
+      </c>
+      <c r="H57" s="1">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>8</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1</v>
+      </c>
+      <c r="H58" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <v>9</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2157,7 +2387,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2181,69 +2411,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>26</v>
+      <c r="A1" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="18"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+    </row>
+    <row r="2" spans="1:16" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-    </row>
-    <row r="2" spans="1:16" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="6">
         <f>-180+M3</f>
@@ -2268,10 +2498,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="M3" s="6">
         <v>0</v>
@@ -2282,13 +2512,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="6">
         <f>180+M5</f>
@@ -2313,10 +2543,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="M4" s="6">
         <v>90</v>
@@ -2327,13 +2557,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D5" s="6">
         <f>-180+M4</f>
@@ -2358,86 +2588,86 @@
         <v>90</v>
       </c>
       <c r="J5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="17">
+        <v>-6.556511E-9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="19">
-        <v>-6.556511E-9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-    </row>
-    <row r="8" spans="1:16" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="N8" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="L9" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" s="21">
-        <v>0</v>
-      </c>
-      <c r="N9" s="21">
+      <c r="M9" s="19">
+        <v>0</v>
+      </c>
+      <c r="N9" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="D10" s="6">
         <f>180+M10</f>
@@ -2462,10 +2692,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="M10" s="6">
         <v>0</v>
@@ -2473,19 +2703,19 @@
       <c r="N10" s="6">
         <v>3.9789209999999998E-2</v>
       </c>
-      <c r="O10" s="22" t="s">
-        <v>46</v>
+      <c r="O10" s="20" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D11" s="6">
         <f>-180+M11</f>
@@ -2510,77 +2740,77 @@
         <v>0</v>
       </c>
       <c r="J11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:16" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="21" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-    </row>
-    <row r="14" spans="1:16" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M14" s="10" t="s">
+      <c r="N14" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6">
         <v>180</v>
@@ -2603,10 +2833,10 @@
         <v>0</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="M15" s="6">
         <v>-100</v>
@@ -2617,13 +2847,13 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="D16" s="6">
         <v>100</v>
@@ -2646,10 +2876,10 @@
         <v>-85</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="M16" s="6">
         <v>0</v>
@@ -2662,74 +2892,74 @@
       <c r="E17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" s="6">
+        <v>0</v>
+      </c>
+      <c r="N17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+    </row>
+    <row r="20" spans="1:15" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="6">
-        <v>0</v>
-      </c>
-      <c r="N17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="L19" s="16" t="s">
+      <c r="E20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-    </row>
-    <row r="20" spans="1:15" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="M20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N20" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="N20" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="6">
         <f>180+M21</f>
@@ -2754,10 +2984,10 @@
         <v>0</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L21" s="9" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="M21" s="6">
         <v>0</v>
@@ -2768,13 +2998,13 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="6">
         <f>-180+M23</f>
@@ -2799,10 +3029,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L22" s="9" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="M22" s="6">
         <v>-90</v>
@@ -2813,13 +3043,13 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D23" s="6">
         <f>-180+M22</f>
@@ -2844,86 +3074,86 @@
         <v>-90</v>
       </c>
       <c r="J23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="6">
+        <v>0</v>
+      </c>
+      <c r="N23" s="17">
+        <v>-6.556511E-9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+    </row>
+    <row r="26" spans="1:15" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="M23" s="6">
-        <v>0</v>
-      </c>
-      <c r="N23" s="19">
-        <v>-6.556511E-9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-    </row>
-    <row r="26" spans="1:15" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="10" t="s">
+      <c r="N26" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L27" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L26" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M26" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N26" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="L27" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="M27" s="21">
-        <v>0</v>
-      </c>
-      <c r="N27" s="21">
+      <c r="M27" s="19">
+        <v>0</v>
+      </c>
+      <c r="N27" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="D28" s="6">
         <f>180+M28</f>
@@ -2948,30 +3178,30 @@
         <v>0</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L28" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="M28" s="21">
-        <v>0</v>
-      </c>
-      <c r="N28" s="21">
+        <v>37</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M28" s="19">
+        <v>0</v>
+      </c>
+      <c r="N28" s="19">
         <v>3.9789209999999998E-2</v>
       </c>
-      <c r="O28" s="22" t="s">
-        <v>46</v>
+      <c r="O28" s="20" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D29" s="6">
         <f>-180+M29</f>
@@ -2996,77 +3226,77 @@
         <v>0</v>
       </c>
       <c r="J29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M29" s="19">
+        <v>0</v>
+      </c>
+      <c r="N29" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L31" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+    </row>
+    <row r="32" spans="1:15" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L29" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M29" s="21">
-        <v>0</v>
-      </c>
-      <c r="N29" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-    </row>
-    <row r="32" spans="1:15" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="10" t="s">
+      <c r="N32" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="N32" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" s="6">
         <v>360</v>
@@ -3089,207 +3319,207 @@
         <v>180</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L33" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="L33" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M33" s="19">
+        <v>80</v>
+      </c>
+      <c r="N33" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="M33" s="21">
-        <v>80</v>
-      </c>
-      <c r="N33" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="21">
+      <c r="D34" s="19">
         <v>-90</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="19">
         <v>270</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="19">
         <v>-1</v>
       </c>
-      <c r="G34" s="21">
-        <v>1</v>
-      </c>
-      <c r="H34" s="21">
+      <c r="G34" s="19">
+        <v>1</v>
+      </c>
+      <c r="H34" s="19">
         <f>+(E34-D34)/(G34-F34)</f>
         <v>180</v>
       </c>
-      <c r="I34" s="21">
+      <c r="I34" s="19">
         <f>+D34-H34*F34</f>
         <v>90</v>
       </c>
-      <c r="J34" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="L34" s="20" t="s">
+      <c r="J34" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L34" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M34" s="19">
+        <v>180</v>
+      </c>
+      <c r="N34" s="19">
+        <v>1.5894140000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="M34" s="21">
-        <v>180</v>
-      </c>
-      <c r="N34" s="21">
-        <v>1.5894140000000001E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="12">
+      <c r="D35" s="11">
         <v>360</v>
       </c>
-      <c r="E35" s="12">
-        <v>0</v>
-      </c>
-      <c r="F35" s="12">
+      <c r="E35" s="11">
+        <v>0</v>
+      </c>
+      <c r="F35" s="11">
         <v>-1</v>
       </c>
-      <c r="G35" s="12">
-        <v>1</v>
-      </c>
-      <c r="H35" s="12">
+      <c r="G35" s="11">
+        <v>1</v>
+      </c>
+      <c r="H35" s="11">
         <f>+(E35-D35)/(G35-F35)</f>
         <v>-180</v>
       </c>
-      <c r="I35" s="12">
+      <c r="I35" s="11">
         <f>+D35-H35*F35</f>
         <v>180</v>
       </c>
-      <c r="J35" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K35" s="12"/>
-      <c r="L35" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M35" s="21">
+      <c r="J35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" s="11"/>
+      <c r="L35" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M35" s="19">
         <v>180</v>
       </c>
-      <c r="N35" s="21">
-        <v>0</v>
-      </c>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12">
+      <c r="N35" s="19">
+        <v>0</v>
+      </c>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11">
         <f>+P34*H35+I35</f>
         <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="12">
+      <c r="A36" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="11">
         <v>-80</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="11">
         <v>-80</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="11">
         <v>-1</v>
       </c>
-      <c r="G36" s="12">
-        <v>1</v>
-      </c>
-      <c r="H36" s="12">
+      <c r="G36" s="11">
+        <v>1</v>
+      </c>
+      <c r="H36" s="11">
         <f>+(E36-D36)/(G36-F36)</f>
         <v>0</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="11">
         <f>+D36-H36*F36</f>
         <v>-80</v>
       </c>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12">
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11">
         <f>+P34*H36+I36+80</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="12">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="11">
         <v>-200</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="11">
         <v>200</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="11">
         <v>-1</v>
       </c>
-      <c r="G37" s="12">
-        <v>1</v>
-      </c>
-      <c r="H37" s="12">
+      <c r="G37" s="11">
+        <v>1</v>
+      </c>
+      <c r="H37" s="11">
         <f>+(E37-D37)/(G37-F37)</f>
         <v>200</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="11">
         <f>+D37-H37*F37</f>
         <v>0</v>
       </c>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12">
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11">
         <f>+P34*H37+I37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="12"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
include lever and door colliders
</commit_message>
<xml_diff>
--- a/Calibration/Formulas.xlsx
+++ b/Calibration/Formulas.xlsx
@@ -16,6 +16,7 @@
     <sheet name="arms" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -416,14 +417,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,7 +980,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2159,8 +2160,8 @@
       <c r="A39" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -2363,7 +2364,7 @@
       <c r="G58" s="1">
         <v>1</v>
       </c>
-      <c r="H58" s="25" t="s">
+      <c r="H58" s="24" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2419,11 +2420,11 @@
       <c r="G1" s="16"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
     </row>
     <row r="2" spans="1:16" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
@@ -2462,8 +2463,8 @@
       <c r="N2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2604,11 +2605,11 @@
       <c r="A7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="8" spans="1:16" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
@@ -2756,11 +2757,11 @@
       <c r="A13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
     </row>
     <row r="14" spans="1:16" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
@@ -2907,11 +2908,11 @@
       <c r="A19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
     </row>
     <row r="20" spans="1:15" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
@@ -3090,11 +3091,11 @@
       <c r="A25" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="L25" s="23" t="s">
+      <c r="L25" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
     </row>
     <row r="26" spans="1:15" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
@@ -3242,11 +3243,11 @@
       <c r="A31" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="L31" s="23" t="s">
+      <c r="L31" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
     </row>
     <row r="32" spans="1:15" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>

</xml_diff>